<commit_message>
fixed BPP Trends on QA
</commit_message>
<xml_diff>
--- a/data/BppTrend/Valid_Import_Files/2020_Trend_Factors_Calculator.xlsx
+++ b/data/BppTrend/Valid_Import_Files/2020_Trend_Factors_Calculator.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sikbhamb\Project\APAS_Automation\qa_automation\data\BppTrend\Valid_Import_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deedeepi1\Automation\qa_automation\data\BppTrend\Valid_Import_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14420" tabRatio="920" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14415" tabRatio="920" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Trends Settings " sheetId="21" r:id="rId1"/>
@@ -979,6 +979,2051 @@
 </styleSheet>
 </file>
 
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX13.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX14.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX15.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX16.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX18.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX19.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX20.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX21.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX22.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX23.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX24.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX25.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX26.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX27.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX28.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX29.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX30.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX31.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX32.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX33.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX34.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX35.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX36.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX37.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX38.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX39.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX40.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX7.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX8.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX9.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9217" name="Control 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9217"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9218" name="Control 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9218"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9219" name="Control 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9219"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9220" name="Control 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9220"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9221" name="Control 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9221"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9222" name="Control 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9222"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9223" name="Control 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9223"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9224" name="Control 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9224"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9225" name="Control 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9225"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9226" name="Control 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9226"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9227" name="Control 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9227"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9228" name="Control 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9228"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9229" name="Control 13" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9229"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9230" name="Control 14" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9230"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9231" name="Control 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9231"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9232" name="Control 16" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9232"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9233" name="Control 17" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9233"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9234" name="Control 18" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9234"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9235" name="Control 19" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9235"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9236" name="Control 20" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9236"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9237" name="Control 21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9237"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9238" name="Control 22" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9238"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9239" name="Control 23" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9239"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9240" name="Control 24" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9240"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9241" name="Control 25" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9241"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9242" name="Control 26" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9242"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9243" name="Control 27" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9243"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9244" name="Control 28" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9244"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9245" name="Control 29" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9245"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>33</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9246" name="Control 30" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9246"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>33</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>34</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9247" name="Control 31" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9247"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>34</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>35</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9248" name="Control 32" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9248"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>35</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9249" name="Control 33" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9249"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>37</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9250" name="Control 34" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9250"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>37</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>38</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9251" name="Control 35" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9251"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>38</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>39</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9252" name="Control 36" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9252"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>39</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>40</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9253" name="Control 37" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9253"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>40</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>41</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9254" name="Control 38" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9254"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>41</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>42</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9255" name="Control 39" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9255"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>42</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>43</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9256" name="Control 40" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9256"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -1285,12 +3330,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1346,14 +3391,14 @@
   </sheetPr>
   <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="23" width="5.7265625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="23" width="5.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -3785,7 +5830,7 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:14">
       <c r="A2" s="17"/>
@@ -4878,7 +6923,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:10">
       <c r="A2" s="41" t="s">
@@ -5558,19 +7603,19 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.1796875" style="21" collapsed="1"/>
-    <col min="3" max="11" width="6.453125" style="21" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.453125" style="22" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="6.453125" style="21" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="6.453125" style="22" customWidth="1" collapsed="1"/>
-    <col min="16" max="23" width="6.453125" style="21" customWidth="1" collapsed="1"/>
-    <col min="24" max="16384" width="9.1796875" style="21" collapsed="1"/>
+    <col min="1" max="1" width="14.7109375" style="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.140625" style="21" collapsed="1"/>
+    <col min="3" max="11" width="6.42578125" style="21" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" style="22" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="6.42578125" style="21" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.42578125" style="22" customWidth="1" collapsed="1"/>
+    <col min="16" max="23" width="6.42578125" style="21" customWidth="1" collapsed="1"/>
+    <col min="24" max="16384" width="9.140625" style="21" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="31" customFormat="1" ht="14">
+    <row r="1" spans="1:23" s="31" customFormat="1" ht="14.25">
       <c r="A1" s="64" t="s">
         <v>5</v>
       </c>
@@ -14139,22 +16184,22 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.26953125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" style="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.26953125" style="21" collapsed="1"/>
-    <col min="3" max="3" width="6.26953125" style="22" customWidth="1" collapsed="1"/>
-    <col min="4" max="11" width="6.26953125" style="21" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.26953125" style="56" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="6.26953125" style="21" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.1796875" style="56" customWidth="1" collapsed="1"/>
-    <col min="16" max="19" width="6.26953125" style="21" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="6.26953125" style="66" collapsed="1"/>
-    <col min="21" max="23" width="6.26953125" style="21" customWidth="1" collapsed="1"/>
-    <col min="24" max="16384" width="6.26953125" style="21" collapsed="1"/>
+    <col min="1" max="1" width="14.140625" style="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.28515625" style="21" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="22" customWidth="1" collapsed="1"/>
+    <col min="4" max="11" width="6.28515625" style="21" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.28515625" style="56" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="6.28515625" style="21" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.140625" style="56" customWidth="1" collapsed="1"/>
+    <col min="16" max="19" width="6.28515625" style="21" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="6.28515625" style="66" collapsed="1"/>
+    <col min="21" max="23" width="6.28515625" style="21" customWidth="1" collapsed="1"/>
+    <col min="24" max="16384" width="6.28515625" style="21" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="32.15" customHeight="1">
+    <row r="1" spans="1:23" ht="32.1" customHeight="1">
       <c r="A1" s="64" t="s">
         <v>7</v>
       </c>
@@ -22719,13 +24764,13 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.81640625" style="21" collapsed="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" style="21" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -23878,13 +25923,13 @@
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.453125" style="21" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" style="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="38" customFormat="1">
@@ -24634,11 +26679,11 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="7" width="10.1796875" style="21" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.1796875" style="21" collapsed="1"/>
+    <col min="1" max="1" width="14.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="7" width="10.140625" style="21" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="21" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -25856,10 +27901,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="15.1796875" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.1796875" style="21" collapsed="1"/>
+    <col min="1" max="4" width="15.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="21" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -26563,716 +28608,720 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1">
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.453125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.453125" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.81640625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="222" width="9.1796875" style="26" collapsed="1"/>
-    <col min="223" max="223" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="224" max="224" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="225" max="225" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="226" max="226" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="227" max="227" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="228" max="228" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="229" max="229" width="9.1796875" style="26" collapsed="1"/>
-    <col min="230" max="230" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="231" max="232" width="9.1796875" style="26" collapsed="1"/>
-    <col min="233" max="233" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="234" max="478" width="9.1796875" style="26" collapsed="1"/>
-    <col min="479" max="479" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="480" max="480" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="481" max="481" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="482" max="482" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="483" max="483" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="484" max="484" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="485" max="485" width="9.1796875" style="26" collapsed="1"/>
-    <col min="486" max="486" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="487" max="488" width="9.1796875" style="26" collapsed="1"/>
-    <col min="489" max="489" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="490" max="734" width="9.1796875" style="26" collapsed="1"/>
-    <col min="735" max="735" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="736" max="736" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="737" max="737" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="738" max="738" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="739" max="739" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="740" max="740" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="741" max="741" width="9.1796875" style="26" collapsed="1"/>
-    <col min="742" max="742" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="743" max="744" width="9.1796875" style="26" collapsed="1"/>
-    <col min="745" max="745" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="746" max="990" width="9.1796875" style="26" collapsed="1"/>
-    <col min="991" max="991" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="992" max="992" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="993" max="993" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="994" max="994" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="995" max="995" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="996" max="996" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="997" max="997" width="9.1796875" style="26" collapsed="1"/>
-    <col min="998" max="998" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="999" max="1000" width="9.1796875" style="26" collapsed="1"/>
-    <col min="1001" max="1001" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="1002" max="1246" width="9.1796875" style="26" collapsed="1"/>
-    <col min="1247" max="1247" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1248" max="1248" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1249" max="1249" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1250" max="1250" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1251" max="1251" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="1252" max="1252" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1253" max="1253" width="9.1796875" style="26" collapsed="1"/>
-    <col min="1254" max="1254" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1255" max="1256" width="9.1796875" style="26" collapsed="1"/>
-    <col min="1257" max="1257" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="1258" max="1502" width="9.1796875" style="26" collapsed="1"/>
-    <col min="1503" max="1503" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1504" max="1504" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1505" max="1505" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1506" max="1506" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1507" max="1507" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="1508" max="1508" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1509" max="1509" width="9.1796875" style="26" collapsed="1"/>
-    <col min="1510" max="1510" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1511" max="1512" width="9.1796875" style="26" collapsed="1"/>
-    <col min="1513" max="1513" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="1514" max="1758" width="9.1796875" style="26" collapsed="1"/>
-    <col min="1759" max="1759" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1760" max="1760" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1761" max="1761" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1762" max="1762" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1763" max="1763" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="1764" max="1764" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1765" max="1765" width="9.1796875" style="26" collapsed="1"/>
-    <col min="1766" max="1766" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1767" max="1768" width="9.1796875" style="26" collapsed="1"/>
-    <col min="1769" max="1769" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="1770" max="2014" width="9.1796875" style="26" collapsed="1"/>
-    <col min="2015" max="2015" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2016" max="2016" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2017" max="2017" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2018" max="2018" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2019" max="2019" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="2020" max="2020" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2021" max="2021" width="9.1796875" style="26" collapsed="1"/>
-    <col min="2022" max="2022" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2023" max="2024" width="9.1796875" style="26" collapsed="1"/>
-    <col min="2025" max="2025" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="2026" max="2270" width="9.1796875" style="26" collapsed="1"/>
-    <col min="2271" max="2271" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2272" max="2272" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2273" max="2273" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2274" max="2274" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2275" max="2275" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="2276" max="2276" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2277" max="2277" width="9.1796875" style="26" collapsed="1"/>
-    <col min="2278" max="2278" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2279" max="2280" width="9.1796875" style="26" collapsed="1"/>
-    <col min="2281" max="2281" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="2282" max="2526" width="9.1796875" style="26" collapsed="1"/>
-    <col min="2527" max="2527" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2528" max="2528" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2529" max="2529" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2530" max="2530" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2531" max="2531" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="2532" max="2532" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2533" max="2533" width="9.1796875" style="26" collapsed="1"/>
-    <col min="2534" max="2534" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2535" max="2536" width="9.1796875" style="26" collapsed="1"/>
-    <col min="2537" max="2537" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="2538" max="2782" width="9.1796875" style="26" collapsed="1"/>
-    <col min="2783" max="2783" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2784" max="2784" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2785" max="2785" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2786" max="2786" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2787" max="2787" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="2788" max="2788" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2789" max="2789" width="9.1796875" style="26" collapsed="1"/>
-    <col min="2790" max="2790" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2791" max="2792" width="9.1796875" style="26" collapsed="1"/>
-    <col min="2793" max="2793" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="2794" max="3038" width="9.1796875" style="26" collapsed="1"/>
-    <col min="3039" max="3039" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3040" max="3040" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3041" max="3041" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3042" max="3042" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3043" max="3043" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="3044" max="3044" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3045" max="3045" width="9.1796875" style="26" collapsed="1"/>
-    <col min="3046" max="3046" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3047" max="3048" width="9.1796875" style="26" collapsed="1"/>
-    <col min="3049" max="3049" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="3050" max="3294" width="9.1796875" style="26" collapsed="1"/>
-    <col min="3295" max="3295" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3296" max="3296" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3297" max="3297" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3298" max="3298" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3299" max="3299" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="3300" max="3300" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3301" max="3301" width="9.1796875" style="26" collapsed="1"/>
-    <col min="3302" max="3302" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3303" max="3304" width="9.1796875" style="26" collapsed="1"/>
-    <col min="3305" max="3305" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="3306" max="3550" width="9.1796875" style="26" collapsed="1"/>
-    <col min="3551" max="3551" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3552" max="3552" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3553" max="3553" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3554" max="3554" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3555" max="3555" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="3556" max="3556" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3557" max="3557" width="9.1796875" style="26" collapsed="1"/>
-    <col min="3558" max="3558" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3559" max="3560" width="9.1796875" style="26" collapsed="1"/>
-    <col min="3561" max="3561" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="3562" max="3806" width="9.1796875" style="26" collapsed="1"/>
-    <col min="3807" max="3807" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3808" max="3808" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3809" max="3809" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3810" max="3810" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3811" max="3811" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="3812" max="3812" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3813" max="3813" width="9.1796875" style="26" collapsed="1"/>
-    <col min="3814" max="3814" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3815" max="3816" width="9.1796875" style="26" collapsed="1"/>
-    <col min="3817" max="3817" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="3818" max="4062" width="9.1796875" style="26" collapsed="1"/>
-    <col min="4063" max="4063" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4064" max="4064" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4065" max="4065" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4066" max="4066" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4067" max="4067" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="4068" max="4068" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4069" max="4069" width="9.1796875" style="26" collapsed="1"/>
-    <col min="4070" max="4070" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4071" max="4072" width="9.1796875" style="26" collapsed="1"/>
-    <col min="4073" max="4073" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="4074" max="4318" width="9.1796875" style="26" collapsed="1"/>
-    <col min="4319" max="4319" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4320" max="4320" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4321" max="4321" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4322" max="4322" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4323" max="4323" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="4324" max="4324" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4325" max="4325" width="9.1796875" style="26" collapsed="1"/>
-    <col min="4326" max="4326" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4327" max="4328" width="9.1796875" style="26" collapsed="1"/>
-    <col min="4329" max="4329" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="4330" max="4574" width="9.1796875" style="26" collapsed="1"/>
-    <col min="4575" max="4575" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4576" max="4576" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4577" max="4577" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4578" max="4578" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4579" max="4579" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="4580" max="4580" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4581" max="4581" width="9.1796875" style="26" collapsed="1"/>
-    <col min="4582" max="4582" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4583" max="4584" width="9.1796875" style="26" collapsed="1"/>
-    <col min="4585" max="4585" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="4586" max="4830" width="9.1796875" style="26" collapsed="1"/>
-    <col min="4831" max="4831" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4832" max="4832" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4833" max="4833" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4834" max="4834" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4835" max="4835" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="4836" max="4836" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4837" max="4837" width="9.1796875" style="26" collapsed="1"/>
-    <col min="4838" max="4838" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4839" max="4840" width="9.1796875" style="26" collapsed="1"/>
-    <col min="4841" max="4841" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="4842" max="5086" width="9.1796875" style="26" collapsed="1"/>
-    <col min="5087" max="5087" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5088" max="5088" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5089" max="5089" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5090" max="5090" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5091" max="5091" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="5092" max="5092" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5093" max="5093" width="9.1796875" style="26" collapsed="1"/>
-    <col min="5094" max="5094" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5095" max="5096" width="9.1796875" style="26" collapsed="1"/>
-    <col min="5097" max="5097" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="5098" max="5342" width="9.1796875" style="26" collapsed="1"/>
-    <col min="5343" max="5343" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5344" max="5344" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5345" max="5345" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5346" max="5346" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5347" max="5347" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="5348" max="5348" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5349" max="5349" width="9.1796875" style="26" collapsed="1"/>
-    <col min="5350" max="5350" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5351" max="5352" width="9.1796875" style="26" collapsed="1"/>
-    <col min="5353" max="5353" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="5354" max="5598" width="9.1796875" style="26" collapsed="1"/>
-    <col min="5599" max="5599" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5600" max="5600" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5601" max="5601" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5602" max="5602" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5603" max="5603" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="5604" max="5604" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5605" max="5605" width="9.1796875" style="26" collapsed="1"/>
-    <col min="5606" max="5606" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5607" max="5608" width="9.1796875" style="26" collapsed="1"/>
-    <col min="5609" max="5609" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="5610" max="5854" width="9.1796875" style="26" collapsed="1"/>
-    <col min="5855" max="5855" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5856" max="5856" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5857" max="5857" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5858" max="5858" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5859" max="5859" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="5860" max="5860" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5861" max="5861" width="9.1796875" style="26" collapsed="1"/>
-    <col min="5862" max="5862" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5863" max="5864" width="9.1796875" style="26" collapsed="1"/>
-    <col min="5865" max="5865" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="5866" max="6110" width="9.1796875" style="26" collapsed="1"/>
-    <col min="6111" max="6111" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6112" max="6112" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6113" max="6113" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6114" max="6114" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6115" max="6115" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="6116" max="6116" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6117" max="6117" width="9.1796875" style="26" collapsed="1"/>
-    <col min="6118" max="6118" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6119" max="6120" width="9.1796875" style="26" collapsed="1"/>
-    <col min="6121" max="6121" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="6122" max="6366" width="9.1796875" style="26" collapsed="1"/>
-    <col min="6367" max="6367" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6368" max="6368" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6369" max="6369" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6370" max="6370" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6371" max="6371" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="6372" max="6372" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6373" max="6373" width="9.1796875" style="26" collapsed="1"/>
-    <col min="6374" max="6374" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6375" max="6376" width="9.1796875" style="26" collapsed="1"/>
-    <col min="6377" max="6377" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="6378" max="6622" width="9.1796875" style="26" collapsed="1"/>
-    <col min="6623" max="6623" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6624" max="6624" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6625" max="6625" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6626" max="6626" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6627" max="6627" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="6628" max="6628" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6629" max="6629" width="9.1796875" style="26" collapsed="1"/>
-    <col min="6630" max="6630" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6631" max="6632" width="9.1796875" style="26" collapsed="1"/>
-    <col min="6633" max="6633" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="6634" max="6878" width="9.1796875" style="26" collapsed="1"/>
-    <col min="6879" max="6879" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6880" max="6880" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6881" max="6881" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6882" max="6882" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6883" max="6883" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="6884" max="6884" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6885" max="6885" width="9.1796875" style="26" collapsed="1"/>
-    <col min="6886" max="6886" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6887" max="6888" width="9.1796875" style="26" collapsed="1"/>
-    <col min="6889" max="6889" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="6890" max="7134" width="9.1796875" style="26" collapsed="1"/>
-    <col min="7135" max="7135" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7136" max="7136" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7137" max="7137" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7138" max="7138" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7139" max="7139" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="7140" max="7140" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7141" max="7141" width="9.1796875" style="26" collapsed="1"/>
-    <col min="7142" max="7142" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7143" max="7144" width="9.1796875" style="26" collapsed="1"/>
-    <col min="7145" max="7145" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="7146" max="7390" width="9.1796875" style="26" collapsed="1"/>
-    <col min="7391" max="7391" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7392" max="7392" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7393" max="7393" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7394" max="7394" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7395" max="7395" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="7396" max="7396" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7397" max="7397" width="9.1796875" style="26" collapsed="1"/>
-    <col min="7398" max="7398" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7399" max="7400" width="9.1796875" style="26" collapsed="1"/>
-    <col min="7401" max="7401" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="7402" max="7646" width="9.1796875" style="26" collapsed="1"/>
-    <col min="7647" max="7647" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7648" max="7648" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7649" max="7649" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7650" max="7650" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7651" max="7651" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="7652" max="7652" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7653" max="7653" width="9.1796875" style="26" collapsed="1"/>
-    <col min="7654" max="7654" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7655" max="7656" width="9.1796875" style="26" collapsed="1"/>
-    <col min="7657" max="7657" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="7658" max="7902" width="9.1796875" style="26" collapsed="1"/>
-    <col min="7903" max="7903" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7904" max="7904" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7905" max="7905" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7906" max="7906" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7907" max="7907" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="7908" max="7908" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7909" max="7909" width="9.1796875" style="26" collapsed="1"/>
-    <col min="7910" max="7910" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7911" max="7912" width="9.1796875" style="26" collapsed="1"/>
-    <col min="7913" max="7913" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="7914" max="8158" width="9.1796875" style="26" collapsed="1"/>
-    <col min="8159" max="8159" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8160" max="8160" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8161" max="8161" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8162" max="8162" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8163" max="8163" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="8164" max="8164" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8165" max="8165" width="9.1796875" style="26" collapsed="1"/>
-    <col min="8166" max="8166" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8167" max="8168" width="9.1796875" style="26" collapsed="1"/>
-    <col min="8169" max="8169" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="8170" max="8414" width="9.1796875" style="26" collapsed="1"/>
-    <col min="8415" max="8415" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8416" max="8416" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8417" max="8417" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8418" max="8418" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8419" max="8419" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="8420" max="8420" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8421" max="8421" width="9.1796875" style="26" collapsed="1"/>
-    <col min="8422" max="8422" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8423" max="8424" width="9.1796875" style="26" collapsed="1"/>
-    <col min="8425" max="8425" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="8426" max="8670" width="9.1796875" style="26" collapsed="1"/>
-    <col min="8671" max="8671" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8672" max="8672" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8673" max="8673" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8674" max="8674" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8675" max="8675" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="8676" max="8676" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8677" max="8677" width="9.1796875" style="26" collapsed="1"/>
-    <col min="8678" max="8678" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8679" max="8680" width="9.1796875" style="26" collapsed="1"/>
-    <col min="8681" max="8681" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="8682" max="8926" width="9.1796875" style="26" collapsed="1"/>
-    <col min="8927" max="8927" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8928" max="8928" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8929" max="8929" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8930" max="8930" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8931" max="8931" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="8932" max="8932" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8933" max="8933" width="9.1796875" style="26" collapsed="1"/>
-    <col min="8934" max="8934" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8935" max="8936" width="9.1796875" style="26" collapsed="1"/>
-    <col min="8937" max="8937" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="8938" max="9182" width="9.1796875" style="26" collapsed="1"/>
-    <col min="9183" max="9183" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9184" max="9184" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9185" max="9185" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9186" max="9186" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9187" max="9187" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="9188" max="9188" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9189" max="9189" width="9.1796875" style="26" collapsed="1"/>
-    <col min="9190" max="9190" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9191" max="9192" width="9.1796875" style="26" collapsed="1"/>
-    <col min="9193" max="9193" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="9194" max="9438" width="9.1796875" style="26" collapsed="1"/>
-    <col min="9439" max="9439" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9440" max="9440" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9441" max="9441" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9442" max="9442" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9443" max="9443" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="9444" max="9444" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9445" max="9445" width="9.1796875" style="26" collapsed="1"/>
-    <col min="9446" max="9446" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9447" max="9448" width="9.1796875" style="26" collapsed="1"/>
-    <col min="9449" max="9449" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="9450" max="9694" width="9.1796875" style="26" collapsed="1"/>
-    <col min="9695" max="9695" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9696" max="9696" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9697" max="9697" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9698" max="9698" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9699" max="9699" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="9700" max="9700" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9701" max="9701" width="9.1796875" style="26" collapsed="1"/>
-    <col min="9702" max="9702" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9703" max="9704" width="9.1796875" style="26" collapsed="1"/>
-    <col min="9705" max="9705" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="9706" max="9950" width="9.1796875" style="26" collapsed="1"/>
-    <col min="9951" max="9951" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9952" max="9952" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9953" max="9953" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9954" max="9954" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9955" max="9955" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="9956" max="9956" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9957" max="9957" width="9.1796875" style="26" collapsed="1"/>
-    <col min="9958" max="9958" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9959" max="9960" width="9.1796875" style="26" collapsed="1"/>
-    <col min="9961" max="9961" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="9962" max="10206" width="9.1796875" style="26" collapsed="1"/>
-    <col min="10207" max="10207" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10208" max="10208" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10209" max="10209" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10210" max="10210" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10211" max="10211" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="10212" max="10212" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10213" max="10213" width="9.1796875" style="26" collapsed="1"/>
-    <col min="10214" max="10214" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10215" max="10216" width="9.1796875" style="26" collapsed="1"/>
-    <col min="10217" max="10217" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="10218" max="10462" width="9.1796875" style="26" collapsed="1"/>
-    <col min="10463" max="10463" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10464" max="10464" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10465" max="10465" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10466" max="10466" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10467" max="10467" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="10468" max="10468" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10469" max="10469" width="9.1796875" style="26" collapsed="1"/>
-    <col min="10470" max="10470" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10471" max="10472" width="9.1796875" style="26" collapsed="1"/>
-    <col min="10473" max="10473" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="10474" max="10718" width="9.1796875" style="26" collapsed="1"/>
-    <col min="10719" max="10719" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10720" max="10720" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10721" max="10721" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10722" max="10722" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10723" max="10723" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="10724" max="10724" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10725" max="10725" width="9.1796875" style="26" collapsed="1"/>
-    <col min="10726" max="10726" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10727" max="10728" width="9.1796875" style="26" collapsed="1"/>
-    <col min="10729" max="10729" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="10730" max="10974" width="9.1796875" style="26" collapsed="1"/>
-    <col min="10975" max="10975" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10976" max="10976" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10977" max="10977" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10978" max="10978" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10979" max="10979" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="10980" max="10980" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10981" max="10981" width="9.1796875" style="26" collapsed="1"/>
-    <col min="10982" max="10982" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10983" max="10984" width="9.1796875" style="26" collapsed="1"/>
-    <col min="10985" max="10985" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="10986" max="11230" width="9.1796875" style="26" collapsed="1"/>
-    <col min="11231" max="11231" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11232" max="11232" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11233" max="11233" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11234" max="11234" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11235" max="11235" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="11236" max="11236" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11237" max="11237" width="9.1796875" style="26" collapsed="1"/>
-    <col min="11238" max="11238" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11239" max="11240" width="9.1796875" style="26" collapsed="1"/>
-    <col min="11241" max="11241" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="11242" max="11486" width="9.1796875" style="26" collapsed="1"/>
-    <col min="11487" max="11487" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11488" max="11488" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11489" max="11489" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11490" max="11490" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11491" max="11491" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="11492" max="11492" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11493" max="11493" width="9.1796875" style="26" collapsed="1"/>
-    <col min="11494" max="11494" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11495" max="11496" width="9.1796875" style="26" collapsed="1"/>
-    <col min="11497" max="11497" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="11498" max="11742" width="9.1796875" style="26" collapsed="1"/>
-    <col min="11743" max="11743" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11744" max="11744" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11745" max="11745" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11746" max="11746" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11747" max="11747" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="11748" max="11748" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11749" max="11749" width="9.1796875" style="26" collapsed="1"/>
-    <col min="11750" max="11750" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11751" max="11752" width="9.1796875" style="26" collapsed="1"/>
-    <col min="11753" max="11753" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="11754" max="11998" width="9.1796875" style="26" collapsed="1"/>
-    <col min="11999" max="11999" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12000" max="12000" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12001" max="12001" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12002" max="12002" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12003" max="12003" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="12004" max="12004" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12005" max="12005" width="9.1796875" style="26" collapsed="1"/>
-    <col min="12006" max="12006" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12007" max="12008" width="9.1796875" style="26" collapsed="1"/>
-    <col min="12009" max="12009" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="12010" max="12254" width="9.1796875" style="26" collapsed="1"/>
-    <col min="12255" max="12255" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12256" max="12256" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12257" max="12257" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12258" max="12258" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12259" max="12259" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="12260" max="12260" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12261" max="12261" width="9.1796875" style="26" collapsed="1"/>
-    <col min="12262" max="12262" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12263" max="12264" width="9.1796875" style="26" collapsed="1"/>
-    <col min="12265" max="12265" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="12266" max="12510" width="9.1796875" style="26" collapsed="1"/>
-    <col min="12511" max="12511" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12512" max="12512" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12513" max="12513" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12514" max="12514" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12515" max="12515" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="12516" max="12516" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12517" max="12517" width="9.1796875" style="26" collapsed="1"/>
-    <col min="12518" max="12518" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12519" max="12520" width="9.1796875" style="26" collapsed="1"/>
-    <col min="12521" max="12521" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="12522" max="12766" width="9.1796875" style="26" collapsed="1"/>
-    <col min="12767" max="12767" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12768" max="12768" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12769" max="12769" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12770" max="12770" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12771" max="12771" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="12772" max="12772" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12773" max="12773" width="9.1796875" style="26" collapsed="1"/>
-    <col min="12774" max="12774" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12775" max="12776" width="9.1796875" style="26" collapsed="1"/>
-    <col min="12777" max="12777" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="12778" max="13022" width="9.1796875" style="26" collapsed="1"/>
-    <col min="13023" max="13023" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13024" max="13024" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13025" max="13025" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13026" max="13026" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13027" max="13027" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="13028" max="13028" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13029" max="13029" width="9.1796875" style="26" collapsed="1"/>
-    <col min="13030" max="13030" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13031" max="13032" width="9.1796875" style="26" collapsed="1"/>
-    <col min="13033" max="13033" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="13034" max="13278" width="9.1796875" style="26" collapsed="1"/>
-    <col min="13279" max="13279" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13280" max="13280" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13281" max="13281" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13282" max="13282" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13283" max="13283" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="13284" max="13284" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13285" max="13285" width="9.1796875" style="26" collapsed="1"/>
-    <col min="13286" max="13286" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13287" max="13288" width="9.1796875" style="26" collapsed="1"/>
-    <col min="13289" max="13289" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="13290" max="13534" width="9.1796875" style="26" collapsed="1"/>
-    <col min="13535" max="13535" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13536" max="13536" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13537" max="13537" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13538" max="13538" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13539" max="13539" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="13540" max="13540" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13541" max="13541" width="9.1796875" style="26" collapsed="1"/>
-    <col min="13542" max="13542" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13543" max="13544" width="9.1796875" style="26" collapsed="1"/>
-    <col min="13545" max="13545" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="13546" max="13790" width="9.1796875" style="26" collapsed="1"/>
-    <col min="13791" max="13791" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13792" max="13792" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13793" max="13793" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13794" max="13794" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13795" max="13795" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="13796" max="13796" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13797" max="13797" width="9.1796875" style="26" collapsed="1"/>
-    <col min="13798" max="13798" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13799" max="13800" width="9.1796875" style="26" collapsed="1"/>
-    <col min="13801" max="13801" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="13802" max="14046" width="9.1796875" style="26" collapsed="1"/>
-    <col min="14047" max="14047" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14048" max="14048" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14049" max="14049" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14050" max="14050" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14051" max="14051" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="14052" max="14052" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14053" max="14053" width="9.1796875" style="26" collapsed="1"/>
-    <col min="14054" max="14054" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14055" max="14056" width="9.1796875" style="26" collapsed="1"/>
-    <col min="14057" max="14057" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="14058" max="14302" width="9.1796875" style="26" collapsed="1"/>
-    <col min="14303" max="14303" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14304" max="14304" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14305" max="14305" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14306" max="14306" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14307" max="14307" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="14308" max="14308" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14309" max="14309" width="9.1796875" style="26" collapsed="1"/>
-    <col min="14310" max="14310" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14311" max="14312" width="9.1796875" style="26" collapsed="1"/>
-    <col min="14313" max="14313" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="14314" max="14558" width="9.1796875" style="26" collapsed="1"/>
-    <col min="14559" max="14559" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14560" max="14560" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14561" max="14561" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14562" max="14562" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14563" max="14563" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="14564" max="14564" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14565" max="14565" width="9.1796875" style="26" collapsed="1"/>
-    <col min="14566" max="14566" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14567" max="14568" width="9.1796875" style="26" collapsed="1"/>
-    <col min="14569" max="14569" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="14570" max="14814" width="9.1796875" style="26" collapsed="1"/>
-    <col min="14815" max="14815" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14816" max="14816" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14817" max="14817" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14818" max="14818" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14819" max="14819" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="14820" max="14820" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14821" max="14821" width="9.1796875" style="26" collapsed="1"/>
-    <col min="14822" max="14822" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14823" max="14824" width="9.1796875" style="26" collapsed="1"/>
-    <col min="14825" max="14825" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="14826" max="15070" width="9.1796875" style="26" collapsed="1"/>
-    <col min="15071" max="15071" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15072" max="15072" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15073" max="15073" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15074" max="15074" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15075" max="15075" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="15076" max="15076" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15077" max="15077" width="9.1796875" style="26" collapsed="1"/>
-    <col min="15078" max="15078" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15079" max="15080" width="9.1796875" style="26" collapsed="1"/>
-    <col min="15081" max="15081" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="15082" max="15326" width="9.1796875" style="26" collapsed="1"/>
-    <col min="15327" max="15327" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15328" max="15328" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15329" max="15329" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15330" max="15330" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15331" max="15331" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="15332" max="15332" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15333" max="15333" width="9.1796875" style="26" collapsed="1"/>
-    <col min="15334" max="15334" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15335" max="15336" width="9.1796875" style="26" collapsed="1"/>
-    <col min="15337" max="15337" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="15338" max="15582" width="9.1796875" style="26" collapsed="1"/>
-    <col min="15583" max="15583" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15584" max="15584" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15585" max="15585" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15586" max="15586" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15587" max="15587" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="15588" max="15588" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15589" max="15589" width="9.1796875" style="26" collapsed="1"/>
-    <col min="15590" max="15590" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15591" max="15592" width="9.1796875" style="26" collapsed="1"/>
-    <col min="15593" max="15593" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="15594" max="15838" width="9.1796875" style="26" collapsed="1"/>
-    <col min="15839" max="15839" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15840" max="15840" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15841" max="15841" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15842" max="15842" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15843" max="15843" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="15844" max="15844" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15845" max="15845" width="9.1796875" style="26" collapsed="1"/>
-    <col min="15846" max="15846" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15847" max="15848" width="9.1796875" style="26" collapsed="1"/>
-    <col min="15849" max="15849" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="15850" max="16094" width="9.1796875" style="26" collapsed="1"/>
-    <col min="16095" max="16095" width="18.1796875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16096" max="16096" width="12.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16097" max="16097" width="11.453125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16098" max="16098" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16099" max="16099" width="3.453125" style="26" customWidth="1" collapsed="1"/>
-    <col min="16100" max="16100" width="17.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16101" max="16101" width="9.1796875" style="26" collapsed="1"/>
-    <col min="16102" max="16102" width="14.81640625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16103" max="16104" width="9.1796875" style="26" collapsed="1"/>
-    <col min="16105" max="16105" width="8.81640625" style="26" customWidth="1" collapsed="1"/>
-    <col min="16106" max="16369" width="9.1796875" style="26" collapsed="1"/>
-    <col min="16370" max="16384" width="9.1796875" style="26" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.42578125" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.42578125" style="27" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.85546875" style="26" customWidth="1"/>
+    <col min="6" max="13" width="9.140625" style="26"/>
+    <col min="14" max="212" width="9.140625" style="26" collapsed="1"/>
+    <col min="213" max="213" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="214" max="214" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="215" max="215" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="216" max="216" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="217" max="217" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="218" max="218" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="219" max="219" width="9.140625" style="26" collapsed="1"/>
+    <col min="220" max="220" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="221" max="222" width="9.140625" style="26" collapsed="1"/>
+    <col min="223" max="223" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="224" max="468" width="9.140625" style="26" collapsed="1"/>
+    <col min="469" max="469" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="470" max="470" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="471" max="471" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="472" max="472" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="473" max="473" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="474" max="474" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="475" max="475" width="9.140625" style="26" collapsed="1"/>
+    <col min="476" max="476" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="477" max="478" width="9.140625" style="26" collapsed="1"/>
+    <col min="479" max="479" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="480" max="724" width="9.140625" style="26" collapsed="1"/>
+    <col min="725" max="725" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="726" max="726" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="727" max="727" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="728" max="728" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="729" max="729" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="730" max="730" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="731" max="731" width="9.140625" style="26" collapsed="1"/>
+    <col min="732" max="732" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="733" max="734" width="9.140625" style="26" collapsed="1"/>
+    <col min="735" max="735" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="736" max="980" width="9.140625" style="26" collapsed="1"/>
+    <col min="981" max="981" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="982" max="982" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="983" max="983" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="984" max="984" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="985" max="985" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="986" max="986" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="987" max="987" width="9.140625" style="26" collapsed="1"/>
+    <col min="988" max="988" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="989" max="990" width="9.140625" style="26" collapsed="1"/>
+    <col min="991" max="991" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="992" max="1236" width="9.140625" style="26" collapsed="1"/>
+    <col min="1237" max="1237" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1238" max="1238" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1239" max="1239" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1240" max="1240" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1241" max="1241" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="1242" max="1242" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1243" max="1243" width="9.140625" style="26" collapsed="1"/>
+    <col min="1244" max="1244" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1245" max="1246" width="9.140625" style="26" collapsed="1"/>
+    <col min="1247" max="1247" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="1248" max="1492" width="9.140625" style="26" collapsed="1"/>
+    <col min="1493" max="1493" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1494" max="1494" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1495" max="1495" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1496" max="1496" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1497" max="1497" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="1498" max="1498" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1499" max="1499" width="9.140625" style="26" collapsed="1"/>
+    <col min="1500" max="1500" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1501" max="1502" width="9.140625" style="26" collapsed="1"/>
+    <col min="1503" max="1503" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="1504" max="1748" width="9.140625" style="26" collapsed="1"/>
+    <col min="1749" max="1749" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1750" max="1750" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1751" max="1751" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1752" max="1752" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1753" max="1753" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="1754" max="1754" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1755" max="1755" width="9.140625" style="26" collapsed="1"/>
+    <col min="1756" max="1756" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1757" max="1758" width="9.140625" style="26" collapsed="1"/>
+    <col min="1759" max="1759" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="1760" max="2004" width="9.140625" style="26" collapsed="1"/>
+    <col min="2005" max="2005" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2006" max="2006" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2007" max="2007" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2008" max="2008" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2009" max="2009" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="2010" max="2010" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2011" max="2011" width="9.140625" style="26" collapsed="1"/>
+    <col min="2012" max="2012" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2013" max="2014" width="9.140625" style="26" collapsed="1"/>
+    <col min="2015" max="2015" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="2016" max="2260" width="9.140625" style="26" collapsed="1"/>
+    <col min="2261" max="2261" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2262" max="2262" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2263" max="2263" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2264" max="2264" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2265" max="2265" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="2266" max="2266" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2267" max="2267" width="9.140625" style="26" collapsed="1"/>
+    <col min="2268" max="2268" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2269" max="2270" width="9.140625" style="26" collapsed="1"/>
+    <col min="2271" max="2271" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="2272" max="2516" width="9.140625" style="26" collapsed="1"/>
+    <col min="2517" max="2517" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2518" max="2518" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2519" max="2519" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2520" max="2520" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2521" max="2521" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="2522" max="2522" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2523" max="2523" width="9.140625" style="26" collapsed="1"/>
+    <col min="2524" max="2524" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2525" max="2526" width="9.140625" style="26" collapsed="1"/>
+    <col min="2527" max="2527" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="2528" max="2772" width="9.140625" style="26" collapsed="1"/>
+    <col min="2773" max="2773" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2774" max="2774" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2775" max="2775" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2776" max="2776" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2777" max="2777" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="2778" max="2778" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2779" max="2779" width="9.140625" style="26" collapsed="1"/>
+    <col min="2780" max="2780" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2781" max="2782" width="9.140625" style="26" collapsed="1"/>
+    <col min="2783" max="2783" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="2784" max="3028" width="9.140625" style="26" collapsed="1"/>
+    <col min="3029" max="3029" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3030" max="3030" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3031" max="3031" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3032" max="3032" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3033" max="3033" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="3034" max="3034" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3035" max="3035" width="9.140625" style="26" collapsed="1"/>
+    <col min="3036" max="3036" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3037" max="3038" width="9.140625" style="26" collapsed="1"/>
+    <col min="3039" max="3039" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="3040" max="3284" width="9.140625" style="26" collapsed="1"/>
+    <col min="3285" max="3285" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3286" max="3286" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3287" max="3287" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3288" max="3288" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3289" max="3289" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="3290" max="3290" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3291" max="3291" width="9.140625" style="26" collapsed="1"/>
+    <col min="3292" max="3292" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3293" max="3294" width="9.140625" style="26" collapsed="1"/>
+    <col min="3295" max="3295" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="3296" max="3540" width="9.140625" style="26" collapsed="1"/>
+    <col min="3541" max="3541" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3542" max="3542" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3543" max="3543" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3544" max="3544" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3545" max="3545" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="3546" max="3546" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3547" max="3547" width="9.140625" style="26" collapsed="1"/>
+    <col min="3548" max="3548" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3549" max="3550" width="9.140625" style="26" collapsed="1"/>
+    <col min="3551" max="3551" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="3552" max="3796" width="9.140625" style="26" collapsed="1"/>
+    <col min="3797" max="3797" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3798" max="3798" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3799" max="3799" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3800" max="3800" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3801" max="3801" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="3802" max="3802" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3803" max="3803" width="9.140625" style="26" collapsed="1"/>
+    <col min="3804" max="3804" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3805" max="3806" width="9.140625" style="26" collapsed="1"/>
+    <col min="3807" max="3807" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="3808" max="4052" width="9.140625" style="26" collapsed="1"/>
+    <col min="4053" max="4053" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4054" max="4054" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4055" max="4055" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4056" max="4056" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4057" max="4057" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="4058" max="4058" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4059" max="4059" width="9.140625" style="26" collapsed="1"/>
+    <col min="4060" max="4060" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4061" max="4062" width="9.140625" style="26" collapsed="1"/>
+    <col min="4063" max="4063" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="4064" max="4308" width="9.140625" style="26" collapsed="1"/>
+    <col min="4309" max="4309" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4310" max="4310" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4311" max="4311" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4312" max="4312" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4313" max="4313" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="4314" max="4314" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4315" max="4315" width="9.140625" style="26" collapsed="1"/>
+    <col min="4316" max="4316" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4317" max="4318" width="9.140625" style="26" collapsed="1"/>
+    <col min="4319" max="4319" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="4320" max="4564" width="9.140625" style="26" collapsed="1"/>
+    <col min="4565" max="4565" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4566" max="4566" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4567" max="4567" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4568" max="4568" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4569" max="4569" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="4570" max="4570" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4571" max="4571" width="9.140625" style="26" collapsed="1"/>
+    <col min="4572" max="4572" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4573" max="4574" width="9.140625" style="26" collapsed="1"/>
+    <col min="4575" max="4575" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="4576" max="4820" width="9.140625" style="26" collapsed="1"/>
+    <col min="4821" max="4821" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4822" max="4822" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4823" max="4823" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4824" max="4824" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4825" max="4825" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="4826" max="4826" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4827" max="4827" width="9.140625" style="26" collapsed="1"/>
+    <col min="4828" max="4828" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4829" max="4830" width="9.140625" style="26" collapsed="1"/>
+    <col min="4831" max="4831" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="4832" max="5076" width="9.140625" style="26" collapsed="1"/>
+    <col min="5077" max="5077" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5078" max="5078" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5079" max="5079" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5080" max="5080" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5081" max="5081" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="5082" max="5082" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5083" max="5083" width="9.140625" style="26" collapsed="1"/>
+    <col min="5084" max="5084" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5085" max="5086" width="9.140625" style="26" collapsed="1"/>
+    <col min="5087" max="5087" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="5088" max="5332" width="9.140625" style="26" collapsed="1"/>
+    <col min="5333" max="5333" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5334" max="5334" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5335" max="5335" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5336" max="5336" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5337" max="5337" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="5338" max="5338" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5339" max="5339" width="9.140625" style="26" collapsed="1"/>
+    <col min="5340" max="5340" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5341" max="5342" width="9.140625" style="26" collapsed="1"/>
+    <col min="5343" max="5343" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="5344" max="5588" width="9.140625" style="26" collapsed="1"/>
+    <col min="5589" max="5589" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5590" max="5590" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5591" max="5591" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5592" max="5592" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5593" max="5593" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="5594" max="5594" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5595" max="5595" width="9.140625" style="26" collapsed="1"/>
+    <col min="5596" max="5596" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5597" max="5598" width="9.140625" style="26" collapsed="1"/>
+    <col min="5599" max="5599" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="5600" max="5844" width="9.140625" style="26" collapsed="1"/>
+    <col min="5845" max="5845" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5846" max="5846" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5847" max="5847" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5848" max="5848" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5849" max="5849" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="5850" max="5850" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5851" max="5851" width="9.140625" style="26" collapsed="1"/>
+    <col min="5852" max="5852" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5853" max="5854" width="9.140625" style="26" collapsed="1"/>
+    <col min="5855" max="5855" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="5856" max="6100" width="9.140625" style="26" collapsed="1"/>
+    <col min="6101" max="6101" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6102" max="6102" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6103" max="6103" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6104" max="6104" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6105" max="6105" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="6106" max="6106" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6107" max="6107" width="9.140625" style="26" collapsed="1"/>
+    <col min="6108" max="6108" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6109" max="6110" width="9.140625" style="26" collapsed="1"/>
+    <col min="6111" max="6111" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="6112" max="6356" width="9.140625" style="26" collapsed="1"/>
+    <col min="6357" max="6357" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6358" max="6358" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6359" max="6359" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6360" max="6360" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6361" max="6361" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="6362" max="6362" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6363" max="6363" width="9.140625" style="26" collapsed="1"/>
+    <col min="6364" max="6364" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6365" max="6366" width="9.140625" style="26" collapsed="1"/>
+    <col min="6367" max="6367" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="6368" max="6612" width="9.140625" style="26" collapsed="1"/>
+    <col min="6613" max="6613" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6614" max="6614" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6615" max="6615" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6616" max="6616" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6617" max="6617" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="6618" max="6618" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6619" max="6619" width="9.140625" style="26" collapsed="1"/>
+    <col min="6620" max="6620" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6621" max="6622" width="9.140625" style="26" collapsed="1"/>
+    <col min="6623" max="6623" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="6624" max="6868" width="9.140625" style="26" collapsed="1"/>
+    <col min="6869" max="6869" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6870" max="6870" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6871" max="6871" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6872" max="6872" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6873" max="6873" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="6874" max="6874" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6875" max="6875" width="9.140625" style="26" collapsed="1"/>
+    <col min="6876" max="6876" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6877" max="6878" width="9.140625" style="26" collapsed="1"/>
+    <col min="6879" max="6879" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="6880" max="7124" width="9.140625" style="26" collapsed="1"/>
+    <col min="7125" max="7125" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7126" max="7126" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7127" max="7127" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7128" max="7128" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7129" max="7129" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="7130" max="7130" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7131" max="7131" width="9.140625" style="26" collapsed="1"/>
+    <col min="7132" max="7132" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7133" max="7134" width="9.140625" style="26" collapsed="1"/>
+    <col min="7135" max="7135" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="7136" max="7380" width="9.140625" style="26" collapsed="1"/>
+    <col min="7381" max="7381" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7382" max="7382" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7383" max="7383" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7384" max="7384" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7385" max="7385" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="7386" max="7386" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7387" max="7387" width="9.140625" style="26" collapsed="1"/>
+    <col min="7388" max="7388" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7389" max="7390" width="9.140625" style="26" collapsed="1"/>
+    <col min="7391" max="7391" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="7392" max="7636" width="9.140625" style="26" collapsed="1"/>
+    <col min="7637" max="7637" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7638" max="7638" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7639" max="7639" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7640" max="7640" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7641" max="7641" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="7642" max="7642" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7643" max="7643" width="9.140625" style="26" collapsed="1"/>
+    <col min="7644" max="7644" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7645" max="7646" width="9.140625" style="26" collapsed="1"/>
+    <col min="7647" max="7647" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="7648" max="7892" width="9.140625" style="26" collapsed="1"/>
+    <col min="7893" max="7893" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7894" max="7894" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7895" max="7895" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7896" max="7896" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7897" max="7897" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="7898" max="7898" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7899" max="7899" width="9.140625" style="26" collapsed="1"/>
+    <col min="7900" max="7900" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7901" max="7902" width="9.140625" style="26" collapsed="1"/>
+    <col min="7903" max="7903" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="7904" max="8148" width="9.140625" style="26" collapsed="1"/>
+    <col min="8149" max="8149" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8150" max="8150" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8151" max="8151" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8152" max="8152" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8153" max="8153" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="8154" max="8154" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8155" max="8155" width="9.140625" style="26" collapsed="1"/>
+    <col min="8156" max="8156" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8157" max="8158" width="9.140625" style="26" collapsed="1"/>
+    <col min="8159" max="8159" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="8160" max="8404" width="9.140625" style="26" collapsed="1"/>
+    <col min="8405" max="8405" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8406" max="8406" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8407" max="8407" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8408" max="8408" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8409" max="8409" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="8410" max="8410" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8411" max="8411" width="9.140625" style="26" collapsed="1"/>
+    <col min="8412" max="8412" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8413" max="8414" width="9.140625" style="26" collapsed="1"/>
+    <col min="8415" max="8415" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="8416" max="8660" width="9.140625" style="26" collapsed="1"/>
+    <col min="8661" max="8661" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8662" max="8662" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8663" max="8663" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8664" max="8664" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8665" max="8665" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="8666" max="8666" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8667" max="8667" width="9.140625" style="26" collapsed="1"/>
+    <col min="8668" max="8668" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8669" max="8670" width="9.140625" style="26" collapsed="1"/>
+    <col min="8671" max="8671" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="8672" max="8916" width="9.140625" style="26" collapsed="1"/>
+    <col min="8917" max="8917" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8918" max="8918" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8919" max="8919" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8920" max="8920" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8921" max="8921" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="8922" max="8922" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8923" max="8923" width="9.140625" style="26" collapsed="1"/>
+    <col min="8924" max="8924" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8925" max="8926" width="9.140625" style="26" collapsed="1"/>
+    <col min="8927" max="8927" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="8928" max="9172" width="9.140625" style="26" collapsed="1"/>
+    <col min="9173" max="9173" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9174" max="9174" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9175" max="9175" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9176" max="9176" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9177" max="9177" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="9178" max="9178" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9179" max="9179" width="9.140625" style="26" collapsed="1"/>
+    <col min="9180" max="9180" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9181" max="9182" width="9.140625" style="26" collapsed="1"/>
+    <col min="9183" max="9183" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="9184" max="9428" width="9.140625" style="26" collapsed="1"/>
+    <col min="9429" max="9429" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9430" max="9430" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9431" max="9431" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9432" max="9432" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9433" max="9433" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="9434" max="9434" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9435" max="9435" width="9.140625" style="26" collapsed="1"/>
+    <col min="9436" max="9436" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9437" max="9438" width="9.140625" style="26" collapsed="1"/>
+    <col min="9439" max="9439" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="9440" max="9684" width="9.140625" style="26" collapsed="1"/>
+    <col min="9685" max="9685" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9686" max="9686" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9687" max="9687" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9688" max="9688" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9689" max="9689" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="9690" max="9690" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9691" max="9691" width="9.140625" style="26" collapsed="1"/>
+    <col min="9692" max="9692" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9693" max="9694" width="9.140625" style="26" collapsed="1"/>
+    <col min="9695" max="9695" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="9696" max="9940" width="9.140625" style="26" collapsed="1"/>
+    <col min="9941" max="9941" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9942" max="9942" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9943" max="9943" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9944" max="9944" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9945" max="9945" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="9946" max="9946" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9947" max="9947" width="9.140625" style="26" collapsed="1"/>
+    <col min="9948" max="9948" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9949" max="9950" width="9.140625" style="26" collapsed="1"/>
+    <col min="9951" max="9951" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="9952" max="10196" width="9.140625" style="26" collapsed="1"/>
+    <col min="10197" max="10197" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10198" max="10198" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10199" max="10199" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10200" max="10200" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10201" max="10201" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="10202" max="10202" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10203" max="10203" width="9.140625" style="26" collapsed="1"/>
+    <col min="10204" max="10204" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10205" max="10206" width="9.140625" style="26" collapsed="1"/>
+    <col min="10207" max="10207" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="10208" max="10452" width="9.140625" style="26" collapsed="1"/>
+    <col min="10453" max="10453" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10454" max="10454" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10455" max="10455" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10456" max="10456" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10457" max="10457" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="10458" max="10458" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10459" max="10459" width="9.140625" style="26" collapsed="1"/>
+    <col min="10460" max="10460" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10461" max="10462" width="9.140625" style="26" collapsed="1"/>
+    <col min="10463" max="10463" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="10464" max="10708" width="9.140625" style="26" collapsed="1"/>
+    <col min="10709" max="10709" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10710" max="10710" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10711" max="10711" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10712" max="10712" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10713" max="10713" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="10714" max="10714" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10715" max="10715" width="9.140625" style="26" collapsed="1"/>
+    <col min="10716" max="10716" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10717" max="10718" width="9.140625" style="26" collapsed="1"/>
+    <col min="10719" max="10719" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="10720" max="10964" width="9.140625" style="26" collapsed="1"/>
+    <col min="10965" max="10965" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10966" max="10966" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10967" max="10967" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10968" max="10968" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10969" max="10969" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="10970" max="10970" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10971" max="10971" width="9.140625" style="26" collapsed="1"/>
+    <col min="10972" max="10972" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10973" max="10974" width="9.140625" style="26" collapsed="1"/>
+    <col min="10975" max="10975" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="10976" max="11220" width="9.140625" style="26" collapsed="1"/>
+    <col min="11221" max="11221" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11222" max="11222" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11223" max="11223" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11224" max="11224" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11225" max="11225" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="11226" max="11226" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11227" max="11227" width="9.140625" style="26" collapsed="1"/>
+    <col min="11228" max="11228" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11229" max="11230" width="9.140625" style="26" collapsed="1"/>
+    <col min="11231" max="11231" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="11232" max="11476" width="9.140625" style="26" collapsed="1"/>
+    <col min="11477" max="11477" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11478" max="11478" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11479" max="11479" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11480" max="11480" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11481" max="11481" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="11482" max="11482" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11483" max="11483" width="9.140625" style="26" collapsed="1"/>
+    <col min="11484" max="11484" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11485" max="11486" width="9.140625" style="26" collapsed="1"/>
+    <col min="11487" max="11487" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="11488" max="11732" width="9.140625" style="26" collapsed="1"/>
+    <col min="11733" max="11733" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11734" max="11734" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11735" max="11735" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11736" max="11736" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11737" max="11737" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="11738" max="11738" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11739" max="11739" width="9.140625" style="26" collapsed="1"/>
+    <col min="11740" max="11740" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11741" max="11742" width="9.140625" style="26" collapsed="1"/>
+    <col min="11743" max="11743" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="11744" max="11988" width="9.140625" style="26" collapsed="1"/>
+    <col min="11989" max="11989" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11990" max="11990" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11991" max="11991" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11992" max="11992" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11993" max="11993" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="11994" max="11994" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11995" max="11995" width="9.140625" style="26" collapsed="1"/>
+    <col min="11996" max="11996" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11997" max="11998" width="9.140625" style="26" collapsed="1"/>
+    <col min="11999" max="11999" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="12000" max="12244" width="9.140625" style="26" collapsed="1"/>
+    <col min="12245" max="12245" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12246" max="12246" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12247" max="12247" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12248" max="12248" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12249" max="12249" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="12250" max="12250" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12251" max="12251" width="9.140625" style="26" collapsed="1"/>
+    <col min="12252" max="12252" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12253" max="12254" width="9.140625" style="26" collapsed="1"/>
+    <col min="12255" max="12255" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="12256" max="12500" width="9.140625" style="26" collapsed="1"/>
+    <col min="12501" max="12501" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12502" max="12502" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12503" max="12503" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12504" max="12504" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12505" max="12505" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="12506" max="12506" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12507" max="12507" width="9.140625" style="26" collapsed="1"/>
+    <col min="12508" max="12508" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12509" max="12510" width="9.140625" style="26" collapsed="1"/>
+    <col min="12511" max="12511" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="12512" max="12756" width="9.140625" style="26" collapsed="1"/>
+    <col min="12757" max="12757" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12758" max="12758" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12759" max="12759" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12760" max="12760" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12761" max="12761" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="12762" max="12762" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12763" max="12763" width="9.140625" style="26" collapsed="1"/>
+    <col min="12764" max="12764" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12765" max="12766" width="9.140625" style="26" collapsed="1"/>
+    <col min="12767" max="12767" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="12768" max="13012" width="9.140625" style="26" collapsed="1"/>
+    <col min="13013" max="13013" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13014" max="13014" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13015" max="13015" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13016" max="13016" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13017" max="13017" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="13018" max="13018" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13019" max="13019" width="9.140625" style="26" collapsed="1"/>
+    <col min="13020" max="13020" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13021" max="13022" width="9.140625" style="26" collapsed="1"/>
+    <col min="13023" max="13023" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="13024" max="13268" width="9.140625" style="26" collapsed="1"/>
+    <col min="13269" max="13269" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13270" max="13270" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13271" max="13271" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13272" max="13272" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13273" max="13273" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="13274" max="13274" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13275" max="13275" width="9.140625" style="26" collapsed="1"/>
+    <col min="13276" max="13276" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13277" max="13278" width="9.140625" style="26" collapsed="1"/>
+    <col min="13279" max="13279" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="13280" max="13524" width="9.140625" style="26" collapsed="1"/>
+    <col min="13525" max="13525" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13526" max="13526" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13527" max="13527" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13528" max="13528" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13529" max="13529" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="13530" max="13530" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13531" max="13531" width="9.140625" style="26" collapsed="1"/>
+    <col min="13532" max="13532" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13533" max="13534" width="9.140625" style="26" collapsed="1"/>
+    <col min="13535" max="13535" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="13536" max="13780" width="9.140625" style="26" collapsed="1"/>
+    <col min="13781" max="13781" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13782" max="13782" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13783" max="13783" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13784" max="13784" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13785" max="13785" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="13786" max="13786" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13787" max="13787" width="9.140625" style="26" collapsed="1"/>
+    <col min="13788" max="13788" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13789" max="13790" width="9.140625" style="26" collapsed="1"/>
+    <col min="13791" max="13791" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="13792" max="14036" width="9.140625" style="26" collapsed="1"/>
+    <col min="14037" max="14037" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14038" max="14038" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14039" max="14039" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14040" max="14040" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14041" max="14041" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="14042" max="14042" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14043" max="14043" width="9.140625" style="26" collapsed="1"/>
+    <col min="14044" max="14044" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14045" max="14046" width="9.140625" style="26" collapsed="1"/>
+    <col min="14047" max="14047" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="14048" max="14292" width="9.140625" style="26" collapsed="1"/>
+    <col min="14293" max="14293" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14294" max="14294" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14295" max="14295" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14296" max="14296" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14297" max="14297" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="14298" max="14298" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14299" max="14299" width="9.140625" style="26" collapsed="1"/>
+    <col min="14300" max="14300" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14301" max="14302" width="9.140625" style="26" collapsed="1"/>
+    <col min="14303" max="14303" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="14304" max="14548" width="9.140625" style="26" collapsed="1"/>
+    <col min="14549" max="14549" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14550" max="14550" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14551" max="14551" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14552" max="14552" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14553" max="14553" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="14554" max="14554" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14555" max="14555" width="9.140625" style="26" collapsed="1"/>
+    <col min="14556" max="14556" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14557" max="14558" width="9.140625" style="26" collapsed="1"/>
+    <col min="14559" max="14559" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="14560" max="14804" width="9.140625" style="26" collapsed="1"/>
+    <col min="14805" max="14805" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14806" max="14806" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14807" max="14807" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14808" max="14808" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14809" max="14809" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="14810" max="14810" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14811" max="14811" width="9.140625" style="26" collapsed="1"/>
+    <col min="14812" max="14812" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14813" max="14814" width="9.140625" style="26" collapsed="1"/>
+    <col min="14815" max="14815" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="14816" max="15060" width="9.140625" style="26" collapsed="1"/>
+    <col min="15061" max="15061" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15062" max="15062" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15063" max="15063" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15064" max="15064" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15065" max="15065" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="15066" max="15066" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15067" max="15067" width="9.140625" style="26" collapsed="1"/>
+    <col min="15068" max="15068" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15069" max="15070" width="9.140625" style="26" collapsed="1"/>
+    <col min="15071" max="15071" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="15072" max="15316" width="9.140625" style="26" collapsed="1"/>
+    <col min="15317" max="15317" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15318" max="15318" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15319" max="15319" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15320" max="15320" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15321" max="15321" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="15322" max="15322" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15323" max="15323" width="9.140625" style="26" collapsed="1"/>
+    <col min="15324" max="15324" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15325" max="15326" width="9.140625" style="26" collapsed="1"/>
+    <col min="15327" max="15327" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="15328" max="15572" width="9.140625" style="26" collapsed="1"/>
+    <col min="15573" max="15573" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15574" max="15574" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15575" max="15575" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15576" max="15576" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15577" max="15577" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="15578" max="15578" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15579" max="15579" width="9.140625" style="26" collapsed="1"/>
+    <col min="15580" max="15580" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15581" max="15582" width="9.140625" style="26" collapsed="1"/>
+    <col min="15583" max="15583" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="15584" max="15828" width="9.140625" style="26" collapsed="1"/>
+    <col min="15829" max="15829" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15830" max="15830" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15831" max="15831" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15832" max="15832" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15833" max="15833" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="15834" max="15834" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15835" max="15835" width="9.140625" style="26" collapsed="1"/>
+    <col min="15836" max="15836" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15837" max="15838" width="9.140625" style="26" collapsed="1"/>
+    <col min="15839" max="15839" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="15840" max="16084" width="9.140625" style="26" collapsed="1"/>
+    <col min="16085" max="16085" width="18.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16086" max="16086" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16087" max="16087" width="11.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16088" max="16088" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16089" max="16089" width="3.42578125" style="26" customWidth="1" collapsed="1"/>
+    <col min="16090" max="16090" width="17.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16091" max="16091" width="9.140625" style="26" collapsed="1"/>
+    <col min="16092" max="16092" width="14.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16093" max="16094" width="9.140625" style="26" collapsed="1"/>
+    <col min="16095" max="16095" width="8.85546875" style="26" customWidth="1" collapsed="1"/>
+    <col min="16096" max="16359" width="9.140625" style="26" collapsed="1"/>
+    <col min="16360" max="16384" width="9.140625" style="26" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15">
@@ -27899,6 +29948,1010 @@
     <oddHeader>&amp;CCPI Worksheet</oddHeader>
     <oddFooter>&amp;A</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9256" r:id="rId4" name="Control 40">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>42</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>43</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9256" r:id="rId4" name="Control 40"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9255" r:id="rId6" name="Control 39">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>42</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9255" r:id="rId6" name="Control 39"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9254" r:id="rId8" name="Control 38">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9254" r:id="rId8" name="Control 38"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9253" r:id="rId9" name="Control 37">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9253" r:id="rId9" name="Control 37"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9252" r:id="rId10" name="Control 36">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9252" r:id="rId10" name="Control 36"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9251" r:id="rId11" name="Control 35">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9251" r:id="rId11" name="Control 35"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9250" r:id="rId12" name="Control 34">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9250" r:id="rId12" name="Control 34"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9249" r:id="rId13" name="Control 33">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9249" r:id="rId13" name="Control 33"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9248" r:id="rId14" name="Control 32">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9248" r:id="rId14" name="Control 32"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9247" r:id="rId15" name="Control 31">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9247" r:id="rId15" name="Control 31"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9246" r:id="rId16" name="Control 30">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9246" r:id="rId16" name="Control 30"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9245" r:id="rId17" name="Control 29">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9245" r:id="rId17" name="Control 29"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9244" r:id="rId18" name="Control 28">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9244" r:id="rId18" name="Control 28"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9243" r:id="rId19" name="Control 27">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9243" r:id="rId19" name="Control 27"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9242" r:id="rId20" name="Control 26">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9242" r:id="rId20" name="Control 26"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9241" r:id="rId21" name="Control 25">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9241" r:id="rId21" name="Control 25"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9240" r:id="rId22" name="Control 24">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9240" r:id="rId22" name="Control 24"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9239" r:id="rId23" name="Control 23">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9239" r:id="rId23" name="Control 23"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9238" r:id="rId24" name="Control 22">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9238" r:id="rId24" name="Control 22"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9237" r:id="rId25" name="Control 21">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9237" r:id="rId25" name="Control 21"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9236" r:id="rId26" name="Control 20">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9236" r:id="rId26" name="Control 20"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9235" r:id="rId27" name="Control 19">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9235" r:id="rId27" name="Control 19"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9234" r:id="rId28" name="Control 18">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9234" r:id="rId28" name="Control 18"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9233" r:id="rId29" name="Control 17">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9233" r:id="rId29" name="Control 17"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9232" r:id="rId30" name="Control 16">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9232" r:id="rId30" name="Control 16"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9231" r:id="rId31" name="Control 15">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9231" r:id="rId31" name="Control 15"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9230" r:id="rId32" name="Control 14">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9230" r:id="rId32" name="Control 14"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9229" r:id="rId33" name="Control 13">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9229" r:id="rId33" name="Control 13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9228" r:id="rId34" name="Control 12">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9228" r:id="rId34" name="Control 12"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9227" r:id="rId35" name="Control 11">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9227" r:id="rId35" name="Control 11"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9226" r:id="rId36" name="Control 10">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9226" r:id="rId36" name="Control 10"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9225" r:id="rId37" name="Control 9">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9225" r:id="rId37" name="Control 9"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9224" r:id="rId38" name="Control 8">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9224" r:id="rId38" name="Control 8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9223" r:id="rId39" name="Control 7">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9223" r:id="rId39" name="Control 7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9222" r:id="rId40" name="Control 6">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9222" r:id="rId40" name="Control 6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9221" r:id="rId41" name="Control 5">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9221" r:id="rId41" name="Control 5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9220" r:id="rId42" name="Control 4">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9220" r:id="rId42" name="Control 4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9219" r:id="rId43" name="Control 3">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9219" r:id="rId43" name="Control 3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9218" r:id="rId44" name="Control 2">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9218" r:id="rId44" name="Control 2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9217" r:id="rId45" name="Control 1">
+          <controlPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9217" r:id="rId45" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
 
@@ -27910,20 +30963,20 @@
   <dimension ref="A2:Q60"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A11" activeCellId="1" sqref="D3:D42 A11:XFD11"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="5" width="16.7265625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="40.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7265625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.26953125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.7265625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="8.28515625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="15.5">
+    <row r="2" spans="1:17" ht="15.75">
       <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
@@ -27954,7 +31007,7 @@
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
     </row>
-    <row r="3" spans="1:17" s="21" customFormat="1" ht="14.5" customHeight="1">
+    <row r="3" spans="1:17" s="21" customFormat="1" ht="14.45" customHeight="1">
       <c r="A3" s="46">
         <v>2019</v>
       </c>

</xml_diff>